<commit_message>
Fix ritorni caso 444 - 445
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EVOLUSXX/EVOLUS/FSE_UTILS/1.0.0/accreditamento-checklist_V8.2.xlsx
+++ b/GATEWAY/A1#111#EVOLUSXX/EVOLUS/FSE_UTILS/1.0.0/accreditamento-checklist_V8.2.xlsx
@@ -2004,13 +2004,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-19T15:42:51.683Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fd4d90104b7df3bc </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.bb5b7360e08ff3496064bf147226c8d591677ce1b2ace1f24748d857f4f2e61c.960ab88553^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-01-07T11:59:50.873Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202458aad88c06b4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.7acae1a895^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT2</t>
@@ -2021,13 +2021,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-19T16:02:25.341Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bdac9b0724fcca00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.bb5b7360e08ff3496064bf147226c8d591677ce1b2ace1f24748d857f4f2e61c.9f865e0ea9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-01-07T12:08:47.559Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0175d102e17e7ca1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.eefa678ba2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT1</t>
@@ -2161,7 +2161,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2266,6 +2266,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2525,7 +2531,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2762,11 +2768,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3100,7 +3110,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="2" sqref="I223 H228 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3187,7 +3197,7 @@
   <dimension ref="A1:B996"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="2" sqref="I223 H228 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4264,11 +4274,11 @@
   <dimension ref="A1:W809"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F187" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F189" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A187" activeCellId="0" sqref="A187"/>
-      <selection pane="bottomRight" activeCell="I223" activeCellId="0" sqref="I223"/>
+      <selection pane="bottomLeft" activeCell="A189" activeCellId="0" sqref="A189"/>
+      <selection pane="bottomRight" activeCell="H228" activeCellId="1" sqref="I223 H228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12908,7 +12918,7 @@
         <v>522</v>
       </c>
       <c r="F222" s="31" t="n">
-        <v>45645</v>
+        <v>45664</v>
       </c>
       <c r="G222" s="53" t="s">
         <v>523</v>
@@ -12954,8 +12964,8 @@
       <c r="E223" s="51" t="s">
         <v>527</v>
       </c>
-      <c r="F223" s="31" t="n">
-        <v>45645</v>
+      <c r="F223" s="59" t="n">
+        <v>45664</v>
       </c>
       <c r="G223" s="53" t="s">
         <v>528</v>
@@ -17704,7 +17714,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="2" sqref="I223 H228 I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17770,7 +17780,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="2" sqref="I223 H228 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17785,7 +17795,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>543</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -17797,150 +17807,150 @@
       <c r="D1" s="19" t="s">
         <v>545</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="61" t="s">
         <v>546</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="62" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>549</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="64" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="64" t="s">
         <v>551</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C4" s="63" t="n">
+      <c r="C4" s="64" t="n">
         <v>446.447</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="65" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="64" t="s">
         <v>554</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="64" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="64" t="s">
         <v>556</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="65" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="64" t="s">
         <v>558</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="65" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="64" t="s">
         <v>560</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="65" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="64" t="s">
         <v>562</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="65" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="63" t="s">
         <v>564</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="65" t="s">
         <v>565</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="64" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="63" t="s">
         <v>474</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="65" t="s">
         <v>568</v>
       </c>
     </row>
@@ -18914,7 +18924,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="I223 H228 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18925,32 +18935,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="66" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>569</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="66" t="s">
         <v>570</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="66" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="66"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Fix casi di test 444/445
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EVOLUSXX/EVOLUS/FSE_UTILS/1.0.0/accreditamento-checklist_V8.2.xlsx
+++ b/GATEWAY/A1#111#EVOLUSXX/EVOLUS/FSE_UTILS/1.0.0/accreditamento-checklist_V8.2.xlsx
@@ -2004,13 +2004,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2025-01-07T11:59:50.873Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202458aad88c06b4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.7acae1a895^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-01-23T09:25:35.962Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">660b06d9d8d4ed18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.dee5b19038^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT2</t>
@@ -4268,7 +4268,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A189" activeCellId="0" sqref="A189"/>
-      <selection pane="bottomRight" activeCell="H228" activeCellId="0" sqref="H228"/>
+      <selection pane="bottomRight" activeCell="I222" activeCellId="0" sqref="I222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12908,7 +12908,7 @@
         <v>522</v>
       </c>
       <c r="F222" s="31" t="n">
-        <v>45664</v>
+        <v>45680</v>
       </c>
       <c r="G222" s="53" t="s">
         <v>523</v>

</xml_diff>

<commit_message>
Fix ritorni id 30/38
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EVOLUSXX/EVOLUS/FSE_UTILS/1.0.0/accreditamento-checklist_V8.2.xlsx
+++ b/GATEWAY/A1#111#EVOLUSXX/EVOLUS/FSE_UTILS/1.0.0/accreditamento-checklist_V8.2.xlsx
@@ -515,10 +515,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_PSS_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-03T15:44:14Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7fbc859a0f237331 </t>
+    <t xml:space="preserve">2025-01-23T15:28:37.647Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e59a5a6c5a47e6ff</t>
   </si>
   <si>
     <t xml:space="preserve">UNKNOWN_WORKFLOW_ID</t>
@@ -616,10 +616,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_PSS_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-03T15:52:12Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e739a8166addaf6d </t>
+    <t xml:space="preserve">2025-01-23T15:38:01.327Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f4a929e12ac8ee59</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
@@ -2021,13 +2021,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2025-01-07T12:08:47.559Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0175d102e17e7ca1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.eefa678ba2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-01-23T09:44:07.219Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ee4e72b2cd37eb90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.668fbe7de0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT1</t>
@@ -4264,11 +4264,11 @@
   <dimension ref="A1:W809"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F189" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A189" activeCellId="0" sqref="A189"/>
-      <selection pane="bottomRight" activeCell="I222" activeCellId="0" sqref="I222"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5406,7 +5406,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="76.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="n">
         <v>30</v>
       </c>
@@ -5423,12 +5423,12 @@
         <v>97</v>
       </c>
       <c r="F33" s="31" t="n">
-        <v>45629</v>
+        <v>45680</v>
       </c>
       <c r="G33" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="38" t="s">
+      <c r="H33" s="32" t="s">
         <v>103</v>
       </c>
       <c r="I33" s="32" t="s">
@@ -5726,7 +5726,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="94.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="n">
         <v>38</v>
       </c>
@@ -5743,12 +5743,12 @@
         <v>117</v>
       </c>
       <c r="F41" s="31" t="n">
-        <v>45629</v>
+        <v>45680</v>
       </c>
       <c r="G41" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="H41" s="38" t="s">
+      <c r="H41" s="32" t="s">
         <v>121</v>
       </c>
       <c r="I41" s="32" t="s">
@@ -10692,7 +10692,7 @@
       <c r="G173" s="32" t="s">
         <v>375</v>
       </c>
-      <c r="H173" s="38" t="s">
+      <c r="H173" s="32" t="s">
         <v>376</v>
       </c>
       <c r="I173" s="32" t="s">
@@ -10814,7 +10814,7 @@
       <c r="G175" s="32" t="s">
         <v>385</v>
       </c>
-      <c r="H175" s="38" t="s">
+      <c r="H175" s="32" t="s">
         <v>386</v>
       </c>
       <c r="I175" s="38" t="s">
@@ -11058,7 +11058,7 @@
       <c r="G179" s="32" t="s">
         <v>405</v>
       </c>
-      <c r="H179" s="38" t="s">
+      <c r="H179" s="32" t="s">
         <v>406</v>
       </c>
       <c r="I179" s="32" t="s">
@@ -12955,7 +12955,7 @@
         <v>527</v>
       </c>
       <c r="F223" s="31" t="n">
-        <v>45664</v>
+        <v>45680</v>
       </c>
       <c r="G223" s="53" t="s">
         <v>528</v>

</xml_diff>